<commit_message>
Updated data to reflect Lebron breaking scoring record.
</commit_message>
<xml_diff>
--- a/data/Lebron.xlsx
+++ b/data/Lebron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/nba-scoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A785BC-6063-444E-B97F-956F81E74D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2B747E-7DCA-754E-A224-620471A84B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15480" xr2:uid="{CD0D9F31-76EF-EC44-BD1F-E82A3ED21640}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="9">
   <si>
     <t>Game</t>
   </si>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636A3CE4-B9A3-8342-808E-0EA796DE97B8}">
-  <dimension ref="A1:F1408"/>
+  <dimension ref="A1:F1411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1375" workbookViewId="0">
-      <selection activeCell="E1408" sqref="E1408"/>
+    <sheetView tabSelected="1" topLeftCell="A1393" workbookViewId="0">
+      <selection activeCell="D1399" sqref="D1399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -28758,7 +28758,7 @@
         <v>29</v>
       </c>
       <c r="E1348" s="5">
-        <f t="shared" ref="E1348:E1408" si="21">E1347+D1348</f>
+        <f t="shared" ref="E1348:E1411" si="21">E1347+D1348</f>
         <v>36443</v>
       </c>
       <c r="F1348" s="2">
@@ -30022,6 +30022,69 @@
         <v>38299</v>
       </c>
       <c r="F1408" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1409" s="2">
+        <v>1408</v>
+      </c>
+      <c r="B1409" s="4">
+        <v>44959</v>
+      </c>
+      <c r="C1409" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1409" s="5">
+        <v>26</v>
+      </c>
+      <c r="E1409" s="5">
+        <f t="shared" si="21"/>
+        <v>38325</v>
+      </c>
+      <c r="F1409" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1410" s="2">
+        <v>1409</v>
+      </c>
+      <c r="B1410" s="4">
+        <v>44961</v>
+      </c>
+      <c r="C1410" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1410" s="5">
+        <v>27</v>
+      </c>
+      <c r="E1410" s="5">
+        <f t="shared" si="21"/>
+        <v>38352</v>
+      </c>
+      <c r="F1410" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1411" s="2">
+        <v>1410</v>
+      </c>
+      <c r="B1411" s="4">
+        <v>44964</v>
+      </c>
+      <c r="C1411" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1411" s="5">
+        <v>38</v>
+      </c>
+      <c r="E1411" s="5">
+        <f t="shared" si="21"/>
+        <v>38390</v>
+      </c>
+      <c r="F1411" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed some more theme elements around. Still trying to get area plot animation to work, unsuccessful so far.
</commit_message>
<xml_diff>
--- a/data/Lebron.xlsx
+++ b/data/Lebron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgillis/Desktop/Projects/nba-scoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2B747E-7DCA-754E-A224-620471A84B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB24D35A-86B9-C842-B343-4F406DDDFCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15480" xr2:uid="{CD0D9F31-76EF-EC44-BD1F-E82A3ED21640}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="10">
   <si>
     <t>Game</t>
   </si>
@@ -67,12 +67,15 @@
   <si>
     <t>CUMPTS</t>
   </si>
+  <si>
+    <t>CLET</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +94,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636A3CE4-B9A3-8342-808E-0EA796DE97B8}">
   <dimension ref="A1:F1411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1393" workbookViewId="0">
-      <selection activeCell="D1399" sqref="D1399"/>
+    <sheetView tabSelected="1" topLeftCell="A1113" workbookViewId="0">
+      <selection activeCell="D1144" sqref="D1144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -18168,7 +18177,7 @@
         <v>41942</v>
       </c>
       <c r="C844" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D844" s="5">
         <v>17</v>
@@ -18189,7 +18198,7 @@
         <v>41943</v>
       </c>
       <c r="C845" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D845" s="5">
         <v>36</v>
@@ -18210,7 +18219,7 @@
         <v>41947</v>
       </c>
       <c r="C846" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D846" s="5">
         <v>11</v>
@@ -18231,7 +18240,7 @@
         <v>41948</v>
       </c>
       <c r="C847" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D847" s="5">
         <v>31</v>
@@ -18252,7 +18261,7 @@
         <v>41950</v>
       </c>
       <c r="C848" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D848" s="5">
         <v>22</v>
@@ -18273,7 +18282,7 @@
         <v>41953</v>
       </c>
       <c r="C849" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D849" s="5">
         <v>32</v>
@@ -18294,7 +18303,7 @@
         <v>41957</v>
       </c>
       <c r="C850" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D850" s="5">
         <v>41</v>
@@ -18315,7 +18324,7 @@
         <v>41958</v>
       </c>
       <c r="C851" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D851" s="5">
         <v>32</v>
@@ -18336,7 +18345,7 @@
         <v>41960</v>
       </c>
       <c r="C852" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D852" s="5">
         <v>22</v>
@@ -18357,7 +18366,7 @@
         <v>41962</v>
       </c>
       <c r="C853" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D853" s="5">
         <v>15</v>
@@ -18378,7 +18387,7 @@
         <v>41964</v>
       </c>
       <c r="C854" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D854" s="5">
         <v>22</v>
@@ -18399,7 +18408,7 @@
         <v>41965</v>
       </c>
       <c r="C855" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D855" s="5">
         <v>15</v>
@@ -18420,7 +18429,7 @@
         <v>41967</v>
       </c>
       <c r="C856" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D856" s="5">
         <v>29</v>
@@ -18441,7 +18450,7 @@
         <v>41969</v>
       </c>
       <c r="C857" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D857" s="5">
         <v>29</v>
@@ -18462,7 +18471,7 @@
         <v>41972</v>
       </c>
       <c r="C858" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D858" s="5">
         <v>19</v>
@@ -18483,7 +18492,7 @@
         <v>41975</v>
       </c>
       <c r="C859" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D859" s="5">
         <v>26</v>
@@ -18504,7 +18513,7 @@
         <v>41977</v>
       </c>
       <c r="C860" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D860" s="5">
         <v>19</v>
@@ -18525,7 +18534,7 @@
         <v>41978</v>
       </c>
       <c r="C861" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D861" s="5">
         <v>24</v>
@@ -18546,7 +18555,7 @@
         <v>41981</v>
       </c>
       <c r="C862" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D862" s="5">
         <v>18</v>
@@ -18567,7 +18576,7 @@
         <v>41982</v>
       </c>
       <c r="C863" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D863" s="5">
         <v>35</v>
@@ -18588,7 +18597,7 @@
         <v>41985</v>
       </c>
       <c r="C864" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D864" s="5">
         <v>41</v>
@@ -18609,7 +18618,7 @@
         <v>41988</v>
       </c>
       <c r="C865" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D865" s="5">
         <v>27</v>
@@ -18630,7 +18639,7 @@
         <v>41990</v>
       </c>
       <c r="C866" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D866" s="5">
         <v>21</v>
@@ -18651,7 +18660,7 @@
         <v>41992</v>
       </c>
       <c r="C867" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D867" s="5">
         <v>22</v>
@@ -18672,7 +18681,7 @@
         <v>41994</v>
       </c>
       <c r="C868" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D868" s="5">
         <v>25</v>
@@ -18693,7 +18702,7 @@
         <v>41996</v>
       </c>
       <c r="C869" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D869" s="5">
         <v>24</v>
@@ -18714,7 +18723,7 @@
         <v>41998</v>
       </c>
       <c r="C870" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D870" s="5">
         <v>30</v>
@@ -18735,7 +18744,7 @@
         <v>41999</v>
       </c>
       <c r="C871" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D871" s="5">
         <v>29</v>
@@ -18756,7 +18765,7 @@
         <v>42001</v>
       </c>
       <c r="C872" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D872" s="5">
         <v>17</v>
@@ -18777,7 +18786,7 @@
         <v>42017</v>
       </c>
       <c r="C873" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D873" s="5">
         <v>33</v>
@@ -18798,7 +18807,7 @@
         <v>42019</v>
       </c>
       <c r="C874" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D874" s="5">
         <v>36</v>
@@ -18819,7 +18828,7 @@
         <v>42020</v>
       </c>
       <c r="C875" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D875" s="5">
         <v>32</v>
@@ -18840,7 +18849,7 @@
         <v>42023</v>
       </c>
       <c r="C876" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D876" s="5">
         <v>26</v>
@@ -18861,7 +18870,7 @@
         <v>42025</v>
       </c>
       <c r="C877" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D877" s="5">
         <v>26</v>
@@ -18882,7 +18891,7 @@
         <v>42027</v>
       </c>
       <c r="C878" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D878" s="5">
         <v>25</v>
@@ -18903,7 +18912,7 @@
         <v>42029</v>
       </c>
       <c r="C879" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D879" s="5">
         <v>34</v>
@@ -18924,7 +18933,7 @@
         <v>42031</v>
       </c>
       <c r="C880" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D880" s="5">
         <v>32</v>
@@ -18945,7 +18954,7 @@
         <v>42034</v>
       </c>
       <c r="C881" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D881" s="5">
         <v>19</v>
@@ -18966,7 +18975,7 @@
         <v>42035</v>
       </c>
       <c r="C882" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D882" s="5">
         <v>36</v>
@@ -18987,7 +18996,7 @@
         <v>42037</v>
       </c>
       <c r="C883" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D883" s="5">
         <v>18</v>
@@ -19008,7 +19017,7 @@
         <v>42040</v>
       </c>
       <c r="C884" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D884" s="5">
         <v>23</v>
@@ -19029,7 +19038,7 @@
         <v>42041</v>
       </c>
       <c r="C885" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D885" s="5">
         <v>25</v>
@@ -19050,7 +19059,7 @@
         <v>42043</v>
       </c>
       <c r="C886" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D886" s="5">
         <v>22</v>
@@ -19071,7 +19080,7 @@
         <v>42046</v>
       </c>
       <c r="C887" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D887" s="5">
         <v>18</v>
@@ -19092,7 +19101,7 @@
         <v>42047</v>
       </c>
       <c r="C888" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D888" s="5">
         <v>31</v>
@@ -19113,7 +19122,7 @@
         <v>42055</v>
       </c>
       <c r="C889" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D889" s="5">
         <v>28</v>
@@ -19134,7 +19143,7 @@
         <v>42057</v>
       </c>
       <c r="C890" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D890" s="5">
         <v>18</v>
@@ -19155,7 +19164,7 @@
         <v>42059</v>
       </c>
       <c r="C891" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D891" s="5">
         <v>19</v>
@@ -19176,7 +19185,7 @@
         <v>42061</v>
       </c>
       <c r="C892" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D892" s="5">
         <v>42</v>
@@ -19197,7 +19206,7 @@
         <v>42064</v>
       </c>
       <c r="C893" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D893" s="5">
         <v>37</v>
@@ -19218,7 +19227,7 @@
         <v>42066</v>
       </c>
       <c r="C894" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D894" s="5">
         <v>27</v>
@@ -19239,7 +19248,7 @@
         <v>42067</v>
       </c>
       <c r="C895" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D895" s="5">
         <v>29</v>
@@ -19260,7 +19269,7 @@
         <v>42069</v>
       </c>
       <c r="C896" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D896" s="5">
         <v>18</v>
@@ -19281,7 +19290,7 @@
         <v>42070</v>
       </c>
       <c r="C897" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D897" s="5">
         <v>17</v>
@@ -19302,7 +19311,7 @@
         <v>42073</v>
       </c>
       <c r="C898" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D898" s="5">
         <v>27</v>
@@ -19323,7 +19332,7 @@
         <v>42075</v>
       </c>
       <c r="C899" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D899" s="5">
         <v>31</v>
@@ -19344,7 +19353,7 @@
         <v>42078</v>
       </c>
       <c r="C900" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D900" s="5">
         <v>21</v>
@@ -19365,7 +19374,7 @@
         <v>42079</v>
       </c>
       <c r="C901" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D901" s="5">
         <v>26</v>
@@ -19386,7 +19395,7 @@
         <v>42081</v>
       </c>
       <c r="C902" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D902" s="5">
         <v>16</v>
@@ -19407,7 +19416,7 @@
         <v>42083</v>
       </c>
       <c r="C903" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D903" s="5">
         <v>29</v>
@@ -19428,7 +19437,7 @@
         <v>42085</v>
       </c>
       <c r="C904" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D904" s="5">
         <v>28</v>
@@ -19449,7 +19458,7 @@
         <v>42088</v>
       </c>
       <c r="C905" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D905" s="5">
         <v>20</v>
@@ -19470,7 +19479,7 @@
         <v>42090</v>
       </c>
       <c r="C906" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D906" s="5">
         <v>24</v>
@@ -19491,7 +19500,7 @@
         <v>42092</v>
       </c>
       <c r="C907" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D907" s="5">
         <v>20</v>
@@ -19512,7 +19521,7 @@
         <v>42096</v>
       </c>
       <c r="C908" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D908" s="5">
         <v>23</v>
@@ -19533,7 +19542,7 @@
         <v>42099</v>
       </c>
       <c r="C909" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D909" s="5">
         <v>20</v>
@@ -19554,7 +19563,7 @@
         <v>42102</v>
       </c>
       <c r="C910" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D910" s="5">
         <v>21</v>
@@ -19575,7 +19584,7 @@
         <v>42104</v>
       </c>
       <c r="C911" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D911" s="5">
         <v>14</v>
@@ -19596,7 +19605,7 @@
         <v>42107</v>
       </c>
       <c r="C912" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D912" s="5">
         <v>21</v>
@@ -19617,7 +19626,7 @@
         <v>42304</v>
       </c>
       <c r="C913" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D913" s="5">
         <v>25</v>
@@ -19638,7 +19647,7 @@
         <v>42305</v>
       </c>
       <c r="C914" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D914" s="5">
         <v>12</v>
@@ -19659,7 +19668,7 @@
         <v>42307</v>
       </c>
       <c r="C915" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D915" s="5">
         <v>29</v>
@@ -19680,7 +19689,7 @@
         <v>42310</v>
       </c>
       <c r="C916" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D916" s="5">
         <v>22</v>
@@ -19701,7 +19710,7 @@
         <v>42312</v>
       </c>
       <c r="C917" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D917" s="5">
         <v>23</v>
@@ -19722,7 +19731,7 @@
         <v>42314</v>
       </c>
       <c r="C918" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D918" s="5">
         <v>31</v>
@@ -19743,7 +19752,7 @@
         <v>42316</v>
       </c>
       <c r="C919" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D919" s="5">
         <v>29</v>
@@ -19764,7 +19773,7 @@
         <v>42318</v>
       </c>
       <c r="C920" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D920" s="5">
         <v>31</v>
@@ -19785,7 +19794,7 @@
         <v>42321</v>
       </c>
       <c r="C921" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D921" s="5">
         <v>31</v>
@@ -19806,7 +19815,7 @@
         <v>42322</v>
       </c>
       <c r="C922" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D922" s="5">
         <v>37</v>
@@ -19827,7 +19836,7 @@
         <v>42325</v>
       </c>
       <c r="C923" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D923" s="5">
         <v>30</v>
@@ -19848,7 +19857,7 @@
         <v>42327</v>
       </c>
       <c r="C924" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D924" s="5">
         <v>27</v>
@@ -19869,7 +19878,7 @@
         <v>42329</v>
       </c>
       <c r="C925" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D925" s="5">
         <v>19</v>
@@ -19890,7 +19899,7 @@
         <v>42331</v>
       </c>
       <c r="C926" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D926" s="5">
         <v>15</v>
@@ -19911,7 +19920,7 @@
         <v>42333</v>
       </c>
       <c r="C927" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D927" s="5">
         <v>24</v>
@@ -19932,7 +19941,7 @@
         <v>42335</v>
       </c>
       <c r="C928" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D928" s="5">
         <v>25</v>
@@ -19953,7 +19962,7 @@
         <v>42336</v>
       </c>
       <c r="C929" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D929" s="5">
         <v>26</v>
@@ -19974,7 +19983,7 @@
         <v>42339</v>
       </c>
       <c r="C930" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D930" s="5">
         <v>24</v>
@@ -19995,7 +20004,7 @@
         <v>42342</v>
       </c>
       <c r="C931" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D931" s="5">
         <v>37</v>
@@ -20016,7 +20025,7 @@
         <v>42346</v>
       </c>
       <c r="C932" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D932" s="5">
         <v>33</v>
@@ -20037,7 +20046,7 @@
         <v>42349</v>
       </c>
       <c r="C933" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D933" s="5">
         <v>25</v>
@@ -20058,7 +20067,7 @@
         <v>42353</v>
       </c>
       <c r="C934" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D934" s="5">
         <v>24</v>
@@ -20079,7 +20088,7 @@
         <v>42355</v>
       </c>
       <c r="C935" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D935" s="5">
         <v>33</v>
@@ -20100,7 +20109,7 @@
         <v>42358</v>
       </c>
       <c r="C936" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D936" s="5">
         <v>23</v>
@@ -20121,7 +20130,7 @@
         <v>42361</v>
       </c>
       <c r="C937" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D937" s="5">
         <v>24</v>
@@ -20142,7 +20151,7 @@
         <v>42363</v>
       </c>
       <c r="C938" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D938" s="5">
         <v>25</v>
@@ -20163,7 +20172,7 @@
         <v>42364</v>
       </c>
       <c r="C939" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D939" s="5">
         <v>12</v>
@@ -20184,7 +20193,7 @@
         <v>42366</v>
       </c>
       <c r="C940" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D940" s="5">
         <v>14</v>
@@ -20205,7 +20214,7 @@
         <v>42367</v>
       </c>
       <c r="C941" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D941" s="5">
         <v>34</v>
@@ -20226,7 +20235,7 @@
         <v>42371</v>
       </c>
       <c r="C942" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D942" s="5">
         <v>29</v>
@@ -20247,7 +20256,7 @@
         <v>42373</v>
       </c>
       <c r="C943" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D943" s="5">
         <v>20</v>
@@ -20268,7 +20277,7 @@
         <v>42375</v>
       </c>
       <c r="C944" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D944" s="5">
         <v>34</v>
@@ -20289,7 +20298,7 @@
         <v>42377</v>
       </c>
       <c r="C945" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D945" s="5">
         <v>13</v>
@@ -20310,7 +20319,7 @@
         <v>42379</v>
       </c>
       <c r="C946" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D946" s="5">
         <v>37</v>
@@ -20331,7 +20340,7 @@
         <v>42381</v>
       </c>
       <c r="C947" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D947" s="5">
         <v>27</v>
@@ -20352,7 +20361,7 @@
         <v>42383</v>
       </c>
       <c r="C948" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D948" s="5">
         <v>22</v>
@@ -20373,7 +20382,7 @@
         <v>42384</v>
       </c>
       <c r="C949" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D949" s="5">
         <v>19</v>
@@ -20394,7 +20403,7 @@
         <v>42387</v>
       </c>
       <c r="C950" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D950" s="5">
         <v>16</v>
@@ -20415,7 +20424,7 @@
         <v>42389</v>
       </c>
       <c r="C951" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D951" s="5">
         <v>17</v>
@@ -20436,7 +20445,7 @@
         <v>42390</v>
       </c>
       <c r="C952" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D952" s="5">
         <v>22</v>
@@ -20457,7 +20466,7 @@
         <v>42392</v>
       </c>
       <c r="C953" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D953" s="5">
         <v>26</v>
@@ -20478,7 +20487,7 @@
         <v>42394</v>
       </c>
       <c r="C954" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D954" s="5">
         <v>25</v>
@@ -20499,7 +20508,7 @@
         <v>42396</v>
       </c>
       <c r="C955" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D955" s="5">
         <v>21</v>
@@ -20520,7 +20529,7 @@
         <v>42398</v>
       </c>
       <c r="C956" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D956" s="5">
         <v>20</v>
@@ -20541,7 +20550,7 @@
         <v>42399</v>
       </c>
       <c r="C957" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D957" s="5">
         <v>29</v>
@@ -20562,7 +20571,7 @@
         <v>42401</v>
       </c>
       <c r="C958" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D958" s="5">
         <v>24</v>
@@ -20583,7 +20592,7 @@
         <v>42403</v>
       </c>
       <c r="C959" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D959" s="5">
         <v>23</v>
@@ -20604,7 +20613,7 @@
         <v>42405</v>
       </c>
       <c r="C960" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D960" s="5">
         <v>30</v>
@@ -20625,7 +20634,7 @@
         <v>42406</v>
       </c>
       <c r="C961" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D961" s="5">
         <v>27</v>
@@ -20646,7 +20655,7 @@
         <v>42408</v>
       </c>
       <c r="C962" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D962" s="5">
         <v>21</v>
@@ -20667,7 +20676,7 @@
         <v>42410</v>
       </c>
       <c r="C963" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D963" s="5">
         <v>29</v>
@@ -20688,7 +20697,7 @@
         <v>42418</v>
       </c>
       <c r="C964" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D964" s="5">
         <v>25</v>
@@ -20709,7 +20718,7 @@
         <v>42421</v>
       </c>
       <c r="C965" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D965" s="5">
         <v>25</v>
@@ -20730,7 +20739,7 @@
         <v>42422</v>
       </c>
       <c r="C966" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D966" s="5">
         <v>12</v>
@@ -20751,7 +20760,7 @@
         <v>42424</v>
       </c>
       <c r="C967" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D967" s="5">
         <v>23</v>
@@ -20772,7 +20781,7 @@
         <v>42426</v>
       </c>
       <c r="C968" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D968" s="5">
         <v>25</v>
@@ -20793,7 +20802,7 @@
         <v>42429</v>
       </c>
       <c r="C969" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D969" s="5">
         <v>33</v>
@@ -20814,7 +20823,7 @@
         <v>42433</v>
       </c>
       <c r="C970" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D970" s="5">
         <v>19</v>
@@ -20835,7 +20844,7 @@
         <v>42434</v>
       </c>
       <c r="C971" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D971" s="5">
         <v>28</v>
@@ -20856,7 +20865,7 @@
         <v>42436</v>
       </c>
       <c r="C972" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D972" s="5">
         <v>28</v>
@@ -20877,7 +20886,7 @@
         <v>42438</v>
       </c>
       <c r="C973" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D973" s="5">
         <v>25</v>
@@ -20898,7 +20907,7 @@
         <v>42439</v>
       </c>
       <c r="C974" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D974" s="5">
         <v>24</v>
@@ -20919,7 +20928,7 @@
         <v>42442</v>
       </c>
       <c r="C975" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D975" s="5">
         <v>27</v>
@@ -20940,7 +20949,7 @@
         <v>42443</v>
       </c>
       <c r="C976" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D976" s="5">
         <v>23</v>
@@ -20961,7 +20970,7 @@
         <v>42447</v>
       </c>
       <c r="C977" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D977" s="5">
         <v>18</v>
@@ -20982,7 +20991,7 @@
         <v>42448</v>
       </c>
       <c r="C978" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D978" s="5">
         <v>26</v>
@@ -21003,7 +21012,7 @@
         <v>42450</v>
       </c>
       <c r="C979" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D979" s="5">
         <v>33</v>
@@ -21024,7 +21033,7 @@
         <v>42452</v>
       </c>
       <c r="C980" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D980" s="5">
         <v>26</v>
@@ -21045,7 +21054,7 @@
         <v>42453</v>
       </c>
       <c r="C981" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D981" s="5">
         <v>30</v>
@@ -21066,7 +21075,7 @@
         <v>42455</v>
       </c>
       <c r="C982" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D982" s="5">
         <v>27</v>
@@ -21087,7 +21096,7 @@
         <v>42460</v>
       </c>
       <c r="C983" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D983" s="5">
         <v>24</v>
@@ -21108,7 +21117,7 @@
         <v>42461</v>
       </c>
       <c r="C984" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D984" s="5">
         <v>29</v>
@@ -21129,7 +21138,7 @@
         <v>42463</v>
       </c>
       <c r="C985" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D985" s="5">
         <v>31</v>
@@ -21150,7 +21159,7 @@
         <v>42465</v>
       </c>
       <c r="C986" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D986" s="5">
         <v>17</v>
@@ -21171,7 +21180,7 @@
         <v>42469</v>
       </c>
       <c r="C987" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D987" s="5">
         <v>33</v>
@@ -21192,7 +21201,7 @@
         <v>42471</v>
       </c>
       <c r="C988" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D988" s="5">
         <v>34</v>
@@ -21213,7 +21222,7 @@
         <v>42668</v>
       </c>
       <c r="C989" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D989" s="5">
         <v>19</v>
@@ -21234,7 +21243,7 @@
         <v>42671</v>
       </c>
       <c r="C990" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D990" s="5">
         <v>21</v>
@@ -21255,7 +21264,7 @@
         <v>42672</v>
       </c>
       <c r="C991" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D991" s="5">
         <v>23</v>
@@ -21276,7 +21285,7 @@
         <v>42675</v>
       </c>
       <c r="C992" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D992" s="5">
         <v>19</v>
@@ -21297,7 +21306,7 @@
         <v>42677</v>
       </c>
       <c r="C993" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D993" s="5">
         <v>30</v>
@@ -21318,7 +21327,7 @@
         <v>42679</v>
       </c>
       <c r="C994" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D994" s="5">
         <v>25</v>
@@ -21339,7 +21348,7 @@
         <v>42682</v>
       </c>
       <c r="C995" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D995" s="5">
         <v>23</v>
@@ -21360,7 +21369,7 @@
         <v>42685</v>
       </c>
       <c r="C996" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D996" s="5">
         <v>27</v>
@@ -21381,7 +21390,7 @@
         <v>42687</v>
       </c>
       <c r="C997" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D997" s="5">
         <v>19</v>
@@ -21402,7 +21411,7 @@
         <v>42689</v>
       </c>
       <c r="C998" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D998" s="5">
         <v>28</v>
@@ -21423,7 +21432,7 @@
         <v>42692</v>
       </c>
       <c r="C999" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D999" s="5">
         <v>21</v>
@@ -21444,7 +21453,7 @@
         <v>42697</v>
       </c>
       <c r="C1000" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1000" s="5">
         <v>31</v>
@@ -21465,7 +21474,7 @@
         <v>42699</v>
       </c>
       <c r="C1001" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1001" s="5">
         <v>19</v>
@@ -21486,7 +21495,7 @@
         <v>42701</v>
       </c>
       <c r="C1002" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1002" s="5">
         <v>26</v>
@@ -21507,7 +21516,7 @@
         <v>42703</v>
       </c>
       <c r="C1003" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1003" s="5">
         <v>22</v>
@@ -21528,7 +21537,7 @@
         <v>42705</v>
       </c>
       <c r="C1004" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1004" s="5">
         <v>16</v>
@@ -21549,7 +21558,7 @@
         <v>42706</v>
       </c>
       <c r="C1005" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1005" s="5">
         <v>27</v>
@@ -21570,7 +21579,7 @@
         <v>42709</v>
       </c>
       <c r="C1006" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1006" s="5">
         <v>34</v>
@@ -21591,7 +21600,7 @@
         <v>42711</v>
       </c>
       <c r="C1007" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1007" s="5">
         <v>25</v>
@@ -21612,7 +21621,7 @@
         <v>42713</v>
       </c>
       <c r="C1008" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1008" s="5">
         <v>27</v>
@@ -21633,7 +21642,7 @@
         <v>42714</v>
       </c>
       <c r="C1009" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1009" s="5">
         <v>44</v>
@@ -21654,7 +21663,7 @@
         <v>42717</v>
       </c>
       <c r="C1010" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1010" s="5">
         <v>23</v>
@@ -21675,7 +21684,7 @@
         <v>42721</v>
       </c>
       <c r="C1011" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1011" s="5">
         <v>26</v>
@@ -21696,7 +21705,7 @@
         <v>42724</v>
       </c>
       <c r="C1012" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1012" s="5">
         <v>34</v>
@@ -21717,7 +21726,7 @@
         <v>42725</v>
       </c>
       <c r="C1013" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1013" s="5">
         <v>29</v>
@@ -21738,7 +21747,7 @@
         <v>42727</v>
       </c>
       <c r="C1014" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1014" s="5">
         <v>19</v>
@@ -21759,7 +21768,7 @@
         <v>42729</v>
       </c>
       <c r="C1015" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1015" s="5">
         <v>31</v>
@@ -21780,7 +21789,7 @@
         <v>42733</v>
       </c>
       <c r="C1016" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1016" s="5">
         <v>23</v>
@@ -21801,7 +21810,7 @@
         <v>42735</v>
       </c>
       <c r="C1017" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1017" s="5">
         <v>32</v>
@@ -21822,7 +21831,7 @@
         <v>42737</v>
       </c>
       <c r="C1018" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1018" s="5">
         <v>26</v>
@@ -21843,7 +21852,7 @@
         <v>42739</v>
       </c>
       <c r="C1019" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1019" s="5">
         <v>31</v>
@@ -21864,7 +21873,7 @@
         <v>42741</v>
       </c>
       <c r="C1020" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1020" s="5">
         <v>36</v>
@@ -21885,7 +21894,7 @@
         <v>42743</v>
       </c>
       <c r="C1021" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1021" s="5">
         <v>28</v>
@@ -21906,7 +21915,7 @@
         <v>42745</v>
       </c>
       <c r="C1022" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1022" s="5">
         <v>29</v>
@@ -21927,7 +21936,7 @@
         <v>42746</v>
       </c>
       <c r="C1023" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1023" s="5">
         <v>20</v>
@@ -21948,7 +21957,7 @@
         <v>42748</v>
       </c>
       <c r="C1024" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1024" s="5">
         <v>16</v>
@@ -21969,7 +21978,7 @@
         <v>42751</v>
       </c>
       <c r="C1025" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1025" s="5">
         <v>20</v>
@@ -21990,7 +21999,7 @@
         <v>42754</v>
       </c>
       <c r="C1026" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1026" s="5">
         <v>21</v>
@@ -22011,7 +22020,7 @@
         <v>42756</v>
       </c>
       <c r="C1027" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1027" s="5">
         <v>29</v>
@@ -22032,7 +22041,7 @@
         <v>42758</v>
       </c>
       <c r="C1028" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1028" s="5">
         <v>26</v>
@@ -22053,7 +22062,7 @@
         <v>42760</v>
       </c>
       <c r="C1029" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1029" s="5">
         <v>24</v>
@@ -22074,7 +22083,7 @@
         <v>42762</v>
       </c>
       <c r="C1030" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1030" s="5">
         <v>31</v>
@@ -22095,7 +22104,7 @@
         <v>42764</v>
       </c>
       <c r="C1031" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1031" s="5">
         <v>25</v>
@@ -22116,7 +22125,7 @@
         <v>42765</v>
       </c>
       <c r="C1032" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1032" s="5">
         <v>23</v>
@@ -22137,7 +22146,7 @@
         <v>42767</v>
       </c>
       <c r="C1033" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1033" s="5">
         <v>27</v>
@@ -22158,7 +22167,7 @@
         <v>42770</v>
       </c>
       <c r="C1034" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1034" s="5">
         <v>32</v>
@@ -22179,7 +22188,7 @@
         <v>42772</v>
       </c>
       <c r="C1035" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1035" s="5">
         <v>32</v>
@@ -22200,7 +22209,7 @@
         <v>42774</v>
       </c>
       <c r="C1036" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1036" s="5">
         <v>25</v>
@@ -22221,7 +22230,7 @@
         <v>42775</v>
       </c>
       <c r="C1037" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1037" s="5">
         <v>18</v>
@@ -22242,7 +22251,7 @@
         <v>42777</v>
       </c>
       <c r="C1038" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1038" s="5">
         <v>27</v>
@@ -22263,7 +22272,7 @@
         <v>42780</v>
       </c>
       <c r="C1039" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1039" s="5">
         <v>25</v>
@@ -22284,7 +22293,7 @@
         <v>42781</v>
       </c>
       <c r="C1040" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1040" s="5">
         <v>31</v>
@@ -22305,7 +22314,7 @@
         <v>42789</v>
       </c>
       <c r="C1041" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1041" s="5">
         <v>18</v>
@@ -22326,7 +22335,7 @@
         <v>42793</v>
       </c>
       <c r="C1042" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1042" s="5">
         <v>24</v>
@@ -22347,7 +22356,7 @@
         <v>42795</v>
       </c>
       <c r="C1043" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1043" s="5">
         <v>28</v>
@@ -22368,7 +22377,7 @@
         <v>42797</v>
       </c>
       <c r="C1044" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1044" s="5">
         <v>38</v>
@@ -22389,7 +22398,7 @@
         <v>42800</v>
       </c>
       <c r="C1045" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1045" s="5">
         <v>30</v>
@@ -22410,7 +22419,7 @@
         <v>42803</v>
       </c>
       <c r="C1046" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1046" s="5">
         <v>29</v>
@@ -22431,7 +22440,7 @@
         <v>42805</v>
       </c>
       <c r="C1047" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1047" s="5">
         <v>24</v>
@@ -22452,7 +22461,7 @@
         <v>42806</v>
       </c>
       <c r="C1048" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1048" s="5">
         <v>30</v>
@@ -22473,7 +22482,7 @@
         <v>42808</v>
       </c>
       <c r="C1049" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1049" s="5">
         <v>16</v>
@@ -22494,7 +22503,7 @@
         <v>42810</v>
       </c>
       <c r="C1050" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1050" s="5">
         <v>33</v>
@@ -22515,7 +22524,7 @@
         <v>42813</v>
       </c>
       <c r="C1051" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1051" s="5">
         <v>34</v>
@@ -22536,7 +22545,7 @@
         <v>42816</v>
       </c>
       <c r="C1052" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1052" s="5">
         <v>18</v>
@@ -22557,7 +22566,7 @@
         <v>42818</v>
       </c>
       <c r="C1053" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1053" s="5">
         <v>32</v>
@@ -22578,7 +22587,7 @@
         <v>42819</v>
       </c>
       <c r="C1054" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1054" s="5">
         <v>24</v>
@@ -22599,7 +22608,7 @@
         <v>42821</v>
       </c>
       <c r="C1055" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1055" s="5">
         <v>17</v>
@@ -22620,7 +22629,7 @@
         <v>42824</v>
       </c>
       <c r="C1056" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1056" s="5">
         <v>26</v>
@@ -22641,7 +22650,7 @@
         <v>42825</v>
       </c>
       <c r="C1057" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1057" s="5">
         <v>34</v>
@@ -22662,7 +22671,7 @@
         <v>42827</v>
       </c>
       <c r="C1058" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1058" s="5">
         <v>41</v>
@@ -22683,7 +22692,7 @@
         <v>42829</v>
       </c>
       <c r="C1059" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1059" s="5">
         <v>18</v>
@@ -22704,7 +22713,7 @@
         <v>42830</v>
       </c>
       <c r="C1060" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1060" s="5">
         <v>36</v>
@@ -22725,7 +22734,7 @@
         <v>42832</v>
       </c>
       <c r="C1061" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1061" s="5">
         <v>27</v>
@@ -22746,7 +22755,7 @@
         <v>42834</v>
       </c>
       <c r="C1062" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1062" s="5">
         <v>32</v>
@@ -22767,7 +22776,7 @@
         <v>43025</v>
       </c>
       <c r="C1063" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1063" s="5">
         <v>29</v>
@@ -22788,7 +22797,7 @@
         <v>43028</v>
       </c>
       <c r="C1064" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1064" s="5">
         <v>24</v>
@@ -22809,7 +22818,7 @@
         <v>43029</v>
       </c>
       <c r="C1065" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1065" s="5">
         <v>22</v>
@@ -22830,7 +22839,7 @@
         <v>43032</v>
       </c>
       <c r="C1066" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1066" s="5">
         <v>34</v>
@@ -22851,7 +22860,7 @@
         <v>43033</v>
       </c>
       <c r="C1067" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1067" s="5">
         <v>29</v>
@@ -22872,7 +22881,7 @@
         <v>43036</v>
       </c>
       <c r="C1068" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1068" s="5">
         <v>18</v>
@@ -22893,7 +22902,7 @@
         <v>43037</v>
       </c>
       <c r="C1069" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1069" s="5">
         <v>16</v>
@@ -22914,7 +22923,7 @@
         <v>43040</v>
       </c>
       <c r="C1070" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1070" s="5">
         <v>33</v>
@@ -22935,7 +22944,7 @@
         <v>43042</v>
       </c>
       <c r="C1071" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1071" s="5">
         <v>57</v>
@@ -22956,7 +22965,7 @@
         <v>43044</v>
       </c>
       <c r="C1072" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1072" s="5">
         <v>26</v>
@@ -22977,7 +22986,7 @@
         <v>43046</v>
       </c>
       <c r="C1073" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1073" s="5">
         <v>30</v>
@@ -22998,7 +23007,7 @@
         <v>43048</v>
       </c>
       <c r="C1074" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1074" s="5">
         <v>33</v>
@@ -23019,7 +23028,7 @@
         <v>43050</v>
       </c>
       <c r="C1075" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1075" s="5">
         <v>19</v>
@@ -23040,7 +23049,7 @@
         <v>43052</v>
       </c>
       <c r="C1076" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1076" s="5">
         <v>23</v>
@@ -23061,7 +23070,7 @@
         <v>43054</v>
       </c>
       <c r="C1077" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1077" s="5">
         <v>31</v>
@@ -23082,7 +23091,7 @@
         <v>43056</v>
       </c>
       <c r="C1078" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1078" s="5">
         <v>39</v>
@@ -23103,7 +23112,7 @@
         <v>43059</v>
       </c>
       <c r="C1079" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1079" s="5">
         <v>18</v>
@@ -23124,7 +23133,7 @@
         <v>43061</v>
       </c>
       <c r="C1080" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1080" s="5">
         <v>33</v>
@@ -23145,7 +23154,7 @@
         <v>43063</v>
       </c>
       <c r="C1081" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1081" s="5">
         <v>27</v>
@@ -23166,7 +23175,7 @@
         <v>43066</v>
       </c>
       <c r="C1082" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1082" s="5">
         <v>30</v>
@@ -23187,7 +23196,7 @@
         <v>43067</v>
       </c>
       <c r="C1083" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1083" s="5">
         <v>21</v>
@@ -23208,7 +23217,7 @@
         <v>43069</v>
       </c>
       <c r="C1084" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1084" s="5">
         <v>24</v>
@@ -23229,7 +23238,7 @@
         <v>43071</v>
       </c>
       <c r="C1085" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1085" s="5">
         <v>34</v>
@@ -23250,7 +23259,7 @@
         <v>43073</v>
       </c>
       <c r="C1086" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1086" s="5">
         <v>23</v>
@@ -23271,7 +23280,7 @@
         <v>43075</v>
       </c>
       <c r="C1087" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1087" s="5">
         <v>32</v>
@@ -23292,7 +23301,7 @@
         <v>43077</v>
       </c>
       <c r="C1088" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1088" s="5">
         <v>29</v>
@@ -23313,7 +23322,7 @@
         <v>43078</v>
       </c>
       <c r="C1089" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1089" s="5">
         <v>30</v>
@@ -23334,7 +23343,7 @@
         <v>43081</v>
       </c>
       <c r="C1090" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1090" s="5">
         <v>25</v>
@@ -23355,7 +23364,7 @@
         <v>43083</v>
       </c>
       <c r="C1091" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1091" s="5">
         <v>25</v>
@@ -23376,7 +23385,7 @@
         <v>43085</v>
       </c>
       <c r="C1092" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1092" s="5">
         <v>29</v>
@@ -23397,7 +23406,7 @@
         <v>43086</v>
       </c>
       <c r="C1093" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1093" s="5">
         <v>20</v>
@@ -23418,7 +23427,7 @@
         <v>43088</v>
       </c>
       <c r="C1094" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1094" s="5">
         <v>39</v>
@@ -23439,7 +23448,7 @@
         <v>43090</v>
       </c>
       <c r="C1095" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1095" s="5">
         <v>34</v>
@@ -23460,7 +23469,7 @@
         <v>43094</v>
       </c>
       <c r="C1096" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1096" s="5">
         <v>20</v>
@@ -23481,7 +23490,7 @@
         <v>43096</v>
       </c>
       <c r="C1097" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1097" s="5">
         <v>16</v>
@@ -23502,7 +23511,7 @@
         <v>43099</v>
       </c>
       <c r="C1098" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1098" s="5">
         <v>29</v>
@@ -23523,7 +23532,7 @@
         <v>43102</v>
       </c>
       <c r="C1099" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1099" s="5">
         <v>24</v>
@@ -23544,7 +23553,7 @@
         <v>43103</v>
       </c>
       <c r="C1100" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1100" s="5">
         <v>19</v>
@@ -23565,7 +23574,7 @@
         <v>43106</v>
       </c>
       <c r="C1101" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1101" s="5">
         <v>33</v>
@@ -23586,7 +23595,7 @@
         <v>43108</v>
       </c>
       <c r="C1102" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1102" s="5">
         <v>10</v>
@@ -23607,7 +23616,7 @@
         <v>43111</v>
       </c>
       <c r="C1103" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1103" s="5">
         <v>26</v>
@@ -23628,7 +23637,7 @@
         <v>43112</v>
       </c>
       <c r="C1104" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1104" s="5">
         <v>27</v>
@@ -23649,7 +23658,7 @@
         <v>43115</v>
       </c>
       <c r="C1105" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1105" s="5">
         <v>32</v>
@@ -23670,7 +23679,7 @@
         <v>43118</v>
       </c>
       <c r="C1106" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1106" s="5">
         <v>16</v>
@@ -23691,7 +23700,7 @@
         <v>43120</v>
       </c>
       <c r="C1107" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1107" s="5">
         <v>18</v>
@@ -23712,7 +23721,7 @@
         <v>43123</v>
       </c>
       <c r="C1108" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1108" s="5">
         <v>28</v>
@@ -23733,7 +23742,7 @@
         <v>43126</v>
       </c>
       <c r="C1109" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1109" s="5">
         <v>26</v>
@@ -23754,7 +23763,7 @@
         <v>43128</v>
       </c>
       <c r="C1110" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1110" s="5">
         <v>25</v>
@@ -23775,7 +23784,7 @@
         <v>43130</v>
       </c>
       <c r="C1111" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1111" s="5">
         <v>21</v>
@@ -23796,7 +23805,7 @@
         <v>43131</v>
       </c>
       <c r="C1112" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1112" s="5">
         <v>24</v>
@@ -23817,7 +23826,7 @@
         <v>43134</v>
       </c>
       <c r="C1113" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1113" s="5">
         <v>11</v>
@@ -23838,7 +23847,7 @@
         <v>43137</v>
       </c>
       <c r="C1114" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1114" s="5">
         <v>25</v>
@@ -23859,7 +23868,7 @@
         <v>43138</v>
       </c>
       <c r="C1115" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1115" s="5">
         <v>37</v>
@@ -23880,7 +23889,7 @@
         <v>43140</v>
       </c>
       <c r="C1116" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1116" s="5">
         <v>22</v>
@@ -23901,7 +23910,7 @@
         <v>43142</v>
       </c>
       <c r="C1117" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1117" s="5">
         <v>24</v>
@@ -23922,7 +23931,7 @@
         <v>43144</v>
       </c>
       <c r="C1118" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1118" s="5">
         <v>37</v>
@@ -23943,7 +23952,7 @@
         <v>43153</v>
       </c>
       <c r="C1119" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1119" s="5">
         <v>32</v>
@@ -23964,7 +23973,7 @@
         <v>43154</v>
       </c>
       <c r="C1120" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1120" s="5">
         <v>18</v>
@@ -23985,7 +23994,7 @@
         <v>43156</v>
       </c>
       <c r="C1121" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1121" s="5">
         <v>33</v>
@@ -24006,7 +24015,7 @@
         <v>43158</v>
       </c>
       <c r="C1122" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1122" s="5">
         <v>31</v>
@@ -24027,7 +24036,7 @@
         <v>43160</v>
       </c>
       <c r="C1123" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1123" s="5">
         <v>30</v>
@@ -24048,7 +24057,7 @@
         <v>43162</v>
       </c>
       <c r="C1124" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1124" s="5">
         <v>25</v>
@@ -24069,7 +24078,7 @@
         <v>43164</v>
       </c>
       <c r="C1125" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1125" s="5">
         <v>31</v>
@@ -24090,7 +24099,7 @@
         <v>43166</v>
       </c>
       <c r="C1126" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1126" s="5">
         <v>39</v>
@@ -24111,7 +24120,7 @@
         <v>43168</v>
       </c>
       <c r="C1127" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1127" s="5">
         <v>25</v>
@@ -24132,7 +24141,7 @@
         <v>43170</v>
       </c>
       <c r="C1128" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1128" s="5">
         <v>24</v>
@@ -24153,7 +24162,7 @@
         <v>43172</v>
       </c>
       <c r="C1129" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1129" s="5">
         <v>28</v>
@@ -24174,7 +24183,7 @@
         <v>43174</v>
       </c>
       <c r="C1130" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1130" s="5">
         <v>35</v>
@@ -24195,7 +24204,7 @@
         <v>43176</v>
       </c>
       <c r="C1131" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1131" s="5">
         <v>33</v>
@@ -24216,7 +24225,7 @@
         <v>43178</v>
       </c>
       <c r="C1132" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1132" s="5">
         <v>40</v>
@@ -24237,7 +24246,7 @@
         <v>43180</v>
       </c>
       <c r="C1133" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1133" s="5">
         <v>35</v>
@@ -24258,7 +24267,7 @@
         <v>43182</v>
       </c>
       <c r="C1134" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1134" s="5">
         <v>27</v>
@@ -24279,7 +24288,7 @@
         <v>43184</v>
       </c>
       <c r="C1135" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1135" s="5">
         <v>37</v>
@@ -24300,7 +24309,7 @@
         <v>43186</v>
       </c>
       <c r="C1136" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1136" s="5">
         <v>18</v>
@@ -24321,7 +24330,7 @@
         <v>43187</v>
       </c>
       <c r="C1137" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1137" s="5">
         <v>41</v>
@@ -24342,7 +24351,7 @@
         <v>43189</v>
       </c>
       <c r="C1138" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1138" s="5">
         <v>27</v>
@@ -24363,7 +24372,7 @@
         <v>43191</v>
       </c>
       <c r="C1139" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1139" s="5">
         <v>16</v>
@@ -24384,7 +24393,7 @@
         <v>43193</v>
       </c>
       <c r="C1140" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1140" s="5">
         <v>27</v>
@@ -24405,7 +24414,7 @@
         <v>43195</v>
       </c>
       <c r="C1141" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1141" s="5">
         <v>33</v>
@@ -24426,7 +24435,7 @@
         <v>43196</v>
       </c>
       <c r="C1142" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1142" s="5">
         <v>44</v>
@@ -24447,7 +24456,7 @@
         <v>43199</v>
       </c>
       <c r="C1143" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1143" s="5">
         <v>26</v>
@@ -24468,7 +24477,7 @@
         <v>43201</v>
       </c>
       <c r="C1144" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1144" s="5">
         <v>10</v>
@@ -30090,6 +30099,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1576" xr:uid="{636A3CE4-B9A3-8342-808E-0EA796DE97B8}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>